<commit_message>
Finishing c<i and almost c=i
</commit_message>
<xml_diff>
--- a/data/SUT_c=i.xlsx
+++ b/data/SUT_c=i.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maximiko\JuliaEnvironments\RectangularChoice\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B014D40A-4A95-47D8-A741-8BFDB9C0D647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D960BF-480E-46B6-AA58-5D3230C06331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4E0D1365-AAFA-4D31-B34B-F143CEFDB59F}"/>
   </bookViews>
@@ -74,10 +74,10 @@
     <t>f.4</t>
   </si>
   <si>
-    <t>monetary</t>
-  </si>
-  <si>
     <t>physical</t>
+  </si>
+  <si>
+    <t>mixed</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -507,15 +507,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF82BB3-8EDB-4935-BFF4-C9155C21D32B}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -590,15 +588,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B798F1E5-42AA-48E4-A4D5-EF90361D4CD2}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>

</xml_diff>